<commit_message>
Added Courses I need to complete
</commit_message>
<xml_diff>
--- a/Interview_Plan/Interview_Plan.xlsx
+++ b/Interview_Plan/Interview_Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rohit/Github/educative_notes/Interview_Plan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{722DDEE3-202E-7541-ACA5-E0D7D0B1B86D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B64514-90A3-4241-9A8E-BC82372D5C10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31340" yWindow="5100" windowWidth="30220" windowHeight="20860" xr2:uid="{C6A3763A-2806-D64F-A65E-ECB2019F2D05}"/>
+    <workbookView xWindow="-59320" yWindow="2740" windowWidth="38920" windowHeight="28860" xr2:uid="{C6A3763A-2806-D64F-A65E-ECB2019F2D05}"/>
   </bookViews>
   <sheets>
     <sheet name="Datacamp Courses" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Course Names</t>
   </si>
@@ -46,6 +46,81 @@
   </si>
   <si>
     <t>Machine Learning with Tree-Based Models in Python</t>
+  </si>
+  <si>
+    <t>Linear Classifiers in Python</t>
+  </si>
+  <si>
+    <t>Cluster Analysis in Python</t>
+  </si>
+  <si>
+    <t>Extreme Gradient Boosting with XGBoost</t>
+  </si>
+  <si>
+    <t>Preprocessing for Machine Learning in Python</t>
+  </si>
+  <si>
+    <t>Feature Engineering for ML in Python</t>
+  </si>
+  <si>
+    <t>Dimensionality Reduction in Python</t>
+  </si>
+  <si>
+    <t>Model Validation in Python</t>
+  </si>
+  <si>
+    <t>Hypertuning in Python</t>
+  </si>
+  <si>
+    <t>Introduction to Predictive Analytics in Python</t>
+  </si>
+  <si>
+    <t>Ensemble Methods in Python</t>
+  </si>
+  <si>
+    <t>Practicing ML Interview Questions in Python</t>
+  </si>
+  <si>
+    <t>Designing ML Workflows in Python</t>
+  </si>
+  <si>
+    <t>Intermediate Predictive Analytics in Python</t>
+  </si>
+  <si>
+    <t>Unit Testing in Python</t>
+  </si>
+  <si>
+    <t>Software Engineering for Data Scientist in Python</t>
+  </si>
+  <si>
+    <t>Practicing Coding Interview Questions in Python</t>
+  </si>
+  <si>
+    <t>Assessment: ML Fundamentals in Python</t>
+  </si>
+  <si>
+    <t>Assessment: Statistics Fundamentals with Python</t>
+  </si>
+  <si>
+    <t>Assessment: Data Analysis in SQL</t>
+  </si>
+  <si>
+    <t>Introduction to SQL</t>
+  </si>
+  <si>
+    <t>Intermediate SQL</t>
+  </si>
+  <si>
+    <t>Joining Data in SQL</t>
+  </si>
+  <si>
+    <t>EDA in SQL</t>
+  </si>
+  <si>
+    <t>Functions for Manipulating Data in PSQL</t>
+  </si>
+  <si>
+    <t>Completed Date</t>
   </si>
 </sst>
 </file>
@@ -406,35 +481,159 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05571759-95DF-184A-95B2-068806CF5145}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="357" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="45.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed one Datacamp Course
</commit_message>
<xml_diff>
--- a/Interview_Plan/Interview_Plan.xlsx
+++ b/Interview_Plan/Interview_Plan.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rohit/Github/educative_notes/Interview_Plan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B64514-90A3-4241-9A8E-BC82372D5C10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD40EE5D-A484-EC49-80BC-AD7A609E27DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-59320" yWindow="2740" windowWidth="38920" windowHeight="28860" xr2:uid="{C6A3763A-2806-D64F-A65E-ECB2019F2D05}"/>
+    <workbookView xWindow="-24360" yWindow="-780" windowWidth="23040" windowHeight="27860" xr2:uid="{C6A3763A-2806-D64F-A65E-ECB2019F2D05}"/>
   </bookViews>
   <sheets>
     <sheet name="Datacamp Courses" sheetId="1" r:id="rId1"/>
+    <sheet name="Data Structures" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
   <si>
     <t>Course Names</t>
   </si>
@@ -121,6 +122,162 @@
   </si>
   <si>
     <t>Completed Date</t>
+  </si>
+  <si>
+    <t>Arrays in Data Structures</t>
+  </si>
+  <si>
+    <t>Array Operations</t>
+  </si>
+  <si>
+    <t>Array Operations Continued</t>
+  </si>
+  <si>
+    <t>Pointers &amp; Arrays</t>
+  </si>
+  <si>
+    <t>2D Arrays</t>
+  </si>
+  <si>
+    <t>Jenny's Videos</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Pointers in 2D Arrays</t>
+  </si>
+  <si>
+    <t>Linked Lists</t>
+  </si>
+  <si>
+    <t>Types of Linked Lists</t>
+  </si>
+  <si>
+    <t>Arrays vs Linked Lists</t>
+  </si>
+  <si>
+    <t>Linked Lists Implementations</t>
+  </si>
+  <si>
+    <t>Insert a Node in a Singly LL</t>
+  </si>
+  <si>
+    <t>Delete a Node in a Singly LL</t>
+  </si>
+  <si>
+    <t>Length of LL</t>
+  </si>
+  <si>
+    <t>Reverse a Linked List</t>
+  </si>
+  <si>
+    <t>Doubly LL</t>
+  </si>
+  <si>
+    <t>Implement a Doubly LL</t>
+  </si>
+  <si>
+    <t>Insertion in Doubly LL</t>
+  </si>
+  <si>
+    <t>Reverse a Doubly LL</t>
+  </si>
+  <si>
+    <t>Circular LL</t>
+  </si>
+  <si>
+    <t>Implementation of Circular LL</t>
+  </si>
+  <si>
+    <t>CLL insertion</t>
+  </si>
+  <si>
+    <t>CLL deletion</t>
+  </si>
+  <si>
+    <t>Reverse a CLL</t>
+  </si>
+  <si>
+    <t>Stacks</t>
+  </si>
+  <si>
+    <t>Implementation of Stacks using Arrays</t>
+  </si>
+  <si>
+    <t>Implementation of Stacks using Linked Lists</t>
+  </si>
+  <si>
+    <t>Queues</t>
+  </si>
+  <si>
+    <t>Implementation of Queues using arrays</t>
+  </si>
+  <si>
+    <t>Implementation of Queues using LL</t>
+  </si>
+  <si>
+    <t>Circular Queue using Arrays</t>
+  </si>
+  <si>
+    <t>Circular Queue using LL</t>
+  </si>
+  <si>
+    <t>Implementation of Queues using Stack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deque </t>
+  </si>
+  <si>
+    <t>Implementation of Deque using circular queue</t>
+  </si>
+  <si>
+    <t>Implementation of Deque using circular array</t>
+  </si>
+  <si>
+    <t>Trees</t>
+  </si>
+  <si>
+    <t>Binary Trees and its types</t>
+  </si>
+  <si>
+    <t>Binary Tree Implementation</t>
+  </si>
+  <si>
+    <t>Binary Tree using Arrays</t>
+  </si>
+  <si>
+    <t>Binary Tree traversal</t>
+  </si>
+  <si>
+    <t>Binary Search Trees</t>
+  </si>
+  <si>
+    <t>AVL Trees</t>
+  </si>
+  <si>
+    <t>Red Black Tree</t>
+  </si>
+  <si>
+    <t>Splay Trees</t>
+  </si>
+  <si>
+    <t>B-Trees</t>
+  </si>
+  <si>
+    <t>Graphs</t>
+  </si>
+  <si>
+    <t>Search Algorithms</t>
+  </si>
+  <si>
+    <t>Sorting Algorithms</t>
+  </si>
+  <si>
+    <t>Hashing Techniques</t>
+  </si>
+  <si>
+    <t>Dealing with Missing Data in Python</t>
   </si>
 </sst>
 </file>
@@ -164,9 +321,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,10 +639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05571759-95DF-184A-95B2-068806CF5145}">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -576,64 +734,343 @@
         <v>14</v>
       </c>
     </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" s="2">
+        <v>44176</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62543377-AFFC-4844-8A7C-7AE61891B9F8}">
+  <dimension ref="A1:B50"/>
+  <sheetViews>
+    <sheetView zoomScale="161" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="37.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>45</v>
+      </c>
+    </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>